<commit_message>
Revised README with more detailed sample fake data
</commit_message>
<xml_diff>
--- a/sample_export.xlsx
+++ b/sample_export.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kahnmi_m4/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kahnmi_m4/Documents/git/Quicken_Sankey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{695E4403-4DB7-D64B-9825-82238AACA7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25078D23-5E66-4F40-BA27-57F8D9CD64A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="780" windowWidth="33340" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="780" windowWidth="33320" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="2" r:id="rId1"/>
@@ -33,43 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="15">
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Date</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Account</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Category</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="47">
   <si>
     <t>IGNORE</t>
   </si>
@@ -77,49 +41,147 @@
     <t>Account 1</t>
   </si>
   <si>
-    <t>Account 2</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
-    <t>L1:L1L2:L1L2Cat1</t>
-  </si>
-  <si>
-    <t>L1:L1L2:L1L2Cat2</t>
-  </si>
-  <si>
-    <t>L1:L1L2:L1L2Cat3</t>
-  </si>
-  <si>
-    <t>L2:L1</t>
-  </si>
-  <si>
-    <t>L2:L2L2:L2L2C4</t>
-  </si>
-  <si>
-    <t>L2:L2L3:L2L3C5</t>
-  </si>
-  <si>
-    <t>L3:L3L6</t>
-  </si>
-  <si>
-    <t>L2:L2L1:L2L1C4</t>
+    <t>Home:Groceries</t>
+  </si>
+  <si>
+    <t>Home:Restaurants</t>
+  </si>
+  <si>
+    <t>Home:Groceries:Mom</t>
+  </si>
+  <si>
+    <t>Home:Auto:Auto Insurance</t>
+  </si>
+  <si>
+    <t>Insurance: Life Insurance</t>
+  </si>
+  <si>
+    <t>Insurance: Vision Insurance</t>
+  </si>
+  <si>
+    <t>Insurance: Dental Insurance</t>
+  </si>
+  <si>
+    <t>Insurance: Medical Insurance</t>
+  </si>
+  <si>
+    <t>Taxes: Property Taxes</t>
+  </si>
+  <si>
+    <t>Taxes:City Taxes</t>
+  </si>
+  <si>
+    <t>Taxes: SSI Taxes</t>
+  </si>
+  <si>
+    <t>Taxes: Medicare Taxes</t>
+  </si>
+  <si>
+    <t>Insurance: Long Term Care</t>
+  </si>
+  <si>
+    <t>Home:Auto:Repairs</t>
+  </si>
+  <si>
+    <t>Personal:Mobile phone</t>
+  </si>
+  <si>
+    <t>Home:Utilities (Elec/gas)</t>
+  </si>
+  <si>
+    <t>Personal:Entertainment</t>
+  </si>
+  <si>
+    <t>Personal:Gifts</t>
+  </si>
+  <si>
+    <t>Personal:Charity/Donations</t>
+  </si>
+  <si>
+    <t>Personal:Gym</t>
+  </si>
+  <si>
+    <t>Personal:Medical:Doctor</t>
+  </si>
+  <si>
+    <t>Personal:Medical:Pharmacy</t>
+  </si>
+  <si>
+    <t>Personal:Shopping</t>
+  </si>
+  <si>
+    <t>Home:Internet/Cable/Netflix</t>
+  </si>
+  <si>
+    <t>Personal:Travel</t>
+  </si>
+  <si>
+    <t>Account2</t>
+  </si>
+  <si>
+    <t>Account 4</t>
+  </si>
+  <si>
+    <t>Account 3</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Personal:Clothing:Non-work:Joe</t>
+  </si>
+  <si>
+    <t>Personal:Clothing:Work:Joe</t>
+  </si>
+  <si>
+    <t>Personal:Clothing:Non-work:Jane</t>
+  </si>
+  <si>
+    <t>Personal:Clothing:Work:Jane</t>
+  </si>
+  <si>
+    <t>Home:Home Repairs</t>
+  </si>
+  <si>
+    <t>Home:Auto:Car Registration</t>
+  </si>
+  <si>
+    <t>Home:Home Insurance</t>
+  </si>
+  <si>
+    <t>Insurance: Boat Insurance</t>
+  </si>
+  <si>
+    <t>Home:Auto:Gasoline</t>
+  </si>
+  <si>
+    <t>Taxes: Federal Taxes:Estimated Taxes</t>
+  </si>
+  <si>
+    <t>Taxes: State Taxes:Estimated Taxes</t>
+  </si>
+  <si>
+    <t>Taxes: Federal Taxes:Withheld</t>
+  </si>
+  <si>
+    <t>Taxes: State Taxes Withheld</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -454,405 +516,453 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E43"/>
+  <dimension ref="B1:BA85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:D30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="132" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:53" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
+      <c r="X1"/>
+      <c r="Y1"/>
+      <c r="Z1"/>
+      <c r="AA1"/>
+      <c r="AB1"/>
+      <c r="AC1"/>
+      <c r="AD1"/>
+      <c r="AE1"/>
+      <c r="AF1"/>
+      <c r="AG1"/>
+      <c r="AH1"/>
+      <c r="AI1"/>
+      <c r="AJ1"/>
+      <c r="AK1"/>
+      <c r="AL1"/>
+      <c r="AM1"/>
+      <c r="AN1"/>
+      <c r="AO1"/>
+      <c r="AP1"/>
+      <c r="AQ1"/>
+      <c r="AR1"/>
+      <c r="AS1"/>
+      <c r="AT1"/>
+      <c r="AU1"/>
+      <c r="AV1"/>
+      <c r="AW1"/>
+      <c r="AX1"/>
+      <c r="AY1"/>
+      <c r="AZ1"/>
+      <c r="BA1"/>
+    </row>
+    <row r="2" spans="2:53" x14ac:dyDescent="0.2">
+      <c r="B2" s="2">
+        <v>45658</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="2">
-        <v>45713</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
       </c>
       <c r="E2">
         <v>-1500</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
-        <v>45781</v>
+        <v>45659</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>-2200</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
-        <v>45969</v>
+        <v>45660</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>-574</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
-        <v>45969</v>
+        <v>45661</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>-8090.0000000000009</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+        <v>-250</v>
+      </c>
+    </row>
+    <row r="6" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
+        <v>45662</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>-185</v>
+      </c>
+    </row>
+    <row r="7" spans="2:53" x14ac:dyDescent="0.2">
+      <c r="B7" s="2">
+        <v>45663</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>-337</v>
+      </c>
+    </row>
+    <row r="8" spans="2:53" x14ac:dyDescent="0.2">
+      <c r="B8" s="2">
+        <v>45664</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>-52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:53" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <v>45665</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>-130</v>
+      </c>
+    </row>
+    <row r="10" spans="2:53" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
+        <v>45666</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>-293</v>
+      </c>
+    </row>
+    <row r="11" spans="2:53" x14ac:dyDescent="0.2">
+      <c r="B11" s="2">
+        <v>45667</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>-293</v>
+      </c>
+    </row>
+    <row r="12" spans="2:53" x14ac:dyDescent="0.2">
+      <c r="B12" s="2">
+        <v>45668</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>-293</v>
+      </c>
+    </row>
+    <row r="13" spans="2:53" x14ac:dyDescent="0.2">
+      <c r="B13" s="2">
+        <v>45669</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>-195</v>
+      </c>
+    </row>
+    <row r="14" spans="2:53" x14ac:dyDescent="0.2">
+      <c r="B14" s="2">
         <v>45670</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>-5200</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="2">
-        <v>45874</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>-2407</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="2">
-        <v>45918</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>-4579</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="2">
-        <v>45678</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <v>-5281</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="2">
-        <v>45723</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>-5415</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="2">
-        <v>45749</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11">
-        <v>-3810</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="2">
-        <v>45753</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12">
-        <v>-4513</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="2">
-        <v>45762</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>-3614</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="2">
-        <v>45780</v>
-      </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>-4014</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+        <v>-325</v>
+      </c>
+    </row>
+    <row r="15" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
-        <v>45972</v>
+        <v>45671</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>-4567</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+        <v>-209</v>
+      </c>
+    </row>
+    <row r="16" spans="2:53" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
-        <v>45659</v>
+        <v>45672</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>-163</v>
+        <v>-130</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
-        <v>45664</v>
+        <v>45673</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>-227.99999999999997</v>
+        <v>-209</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
-        <v>45667</v>
+        <v>45674</v>
       </c>
       <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
         <v>4</v>
       </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
       <c r="E18">
-        <v>-163</v>
+        <v>-130</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
-        <v>45672</v>
+        <v>45675</v>
       </c>
       <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
       <c r="E19">
-        <v>-227.99999999999997</v>
+        <v>-293</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
-        <v>45674</v>
+        <v>45676</v>
       </c>
       <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
       <c r="E20">
-        <v>-227.99999999999997</v>
+        <v>-293</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
-        <v>45695</v>
+        <v>45677</v>
       </c>
       <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
         <v>4</v>
       </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
       <c r="E21">
-        <v>-260</v>
+        <v>-293</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
-        <v>45702</v>
+        <v>45678</v>
       </c>
       <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
       <c r="E22">
-        <v>-65</v>
+        <v>-195</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
-        <v>45705</v>
+        <v>45679</v>
       </c>
       <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
         <v>4</v>
       </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
       <c r="E23">
-        <v>-98</v>
+        <v>-325</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
-        <v>45709</v>
+        <v>45680</v>
       </c>
       <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
         <v>4</v>
       </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
       <c r="E24">
-        <v>-163</v>
+        <v>-209</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
-        <v>45716</v>
+        <v>45681</v>
       </c>
       <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
       <c r="E25">
-        <v>-358</v>
+        <v>-130</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
-        <v>45723</v>
+        <v>45682</v>
       </c>
       <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
         <v>4</v>
       </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
       <c r="E26">
-        <v>-227.99999999999997</v>
+        <v>-209</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="2">
-        <v>45730</v>
+        <v>45683</v>
       </c>
       <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" t="s">
         <v>4</v>
       </c>
-      <c r="D27" t="s">
-        <v>14</v>
-      </c>
       <c r="E27">
-        <v>-130</v>
+        <v>-202</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
-        <v>45733</v>
+        <v>45684</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E28">
         <v>-293</v>
@@ -860,212 +970,800 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="2">
-        <v>45737</v>
+        <v>45685</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E29">
-        <v>-293</v>
+        <v>-5281</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
-        <v>45744</v>
+        <v>45686</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E30">
-        <v>-293</v>
+        <v>-5415</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
-        <v>45758</v>
+        <v>45687</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E31">
-        <v>-195</v>
+        <v>-3810</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
-        <v>45769</v>
+        <v>45688</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E32">
-        <v>-325</v>
+        <v>-4513</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="2">
-        <v>45771</v>
+        <v>45689</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E33">
-        <v>-209</v>
+        <v>-251</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="2">
-        <v>45773</v>
+        <v>45690</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="E34">
-        <v>-130</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="2">
-        <v>45773</v>
+        <v>45691</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="E35">
-        <v>-209</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="2">
-        <v>45777</v>
+        <v>45692</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="E36">
-        <v>-202</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="2">
-        <v>45779</v>
+        <v>45693</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="E37">
-        <v>-293</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="2">
-        <v>45948</v>
+        <v>45694</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E38">
-        <v>-104</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="2">
-        <v>45955</v>
+        <v>45695</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E39">
-        <v>-130</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="2">
-        <v>45958</v>
+        <v>45696</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E40">
-        <v>-98</v>
+        <v>-1250</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="2">
-        <v>45961</v>
+        <v>45697</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="E41">
-        <v>-195</v>
+        <v>-2200</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="2">
-        <v>45968</v>
+        <v>45698</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E42">
-        <v>-260</v>
+        <v>-1100</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="2">
-        <v>45975</v>
+        <v>45699</v>
       </c>
       <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43">
+        <v>-2210</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>45700</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44">
+        <v>-6210</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>45701</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45">
+        <v>-1423</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>45702</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46">
+        <v>-2240</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>45703</v>
+      </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47">
+        <v>-520</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>45704</v>
+      </c>
+      <c r="C48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48">
+        <v>-1245</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>45705</v>
+      </c>
+      <c r="C49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49">
+        <v>-850</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>45706</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50">
+        <v>-55</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>45707</v>
+      </c>
+      <c r="C51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51">
+        <v>-3812</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>45708</v>
+      </c>
+      <c r="C52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52">
+        <v>-3500</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>45709</v>
+      </c>
+      <c r="C53" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53">
+        <v>-350</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>45710</v>
+      </c>
+      <c r="C54" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54">
+        <v>-250</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>45711</v>
+      </c>
+      <c r="C55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55">
+        <v>-1100</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>45712</v>
+      </c>
+      <c r="C56" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56">
+        <v>-3500</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>45713</v>
+      </c>
+      <c r="C57" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57">
+        <v>-892</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>45714</v>
+      </c>
+      <c r="C58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58">
+        <v>-1400</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>45715</v>
+      </c>
+      <c r="C59" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59">
+        <v>-540</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>45716</v>
+      </c>
+      <c r="C60" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60">
+        <v>-1824</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>45717</v>
+      </c>
+      <c r="C61" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61">
+        <v>-450</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>45718</v>
+      </c>
+      <c r="C62" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62">
+        <v>-540</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>45719</v>
+      </c>
+      <c r="C63" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>45720</v>
+      </c>
+      <c r="C64" t="s">
+        <v>29</v>
+      </c>
+      <c r="D64" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64">
+        <v>-875</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>45721</v>
+      </c>
+      <c r="C65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" t="s">
+        <v>23</v>
+      </c>
+      <c r="E65">
+        <v>-2680</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>45722</v>
+      </c>
+      <c r="C66" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66">
+        <v>-2111</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>45725</v>
+      </c>
+      <c r="C67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D67" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67">
+        <v>-6723</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>45726</v>
+      </c>
+      <c r="C68" t="s">
+        <v>29</v>
+      </c>
+      <c r="D68" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68">
+        <v>-7211</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>45723</v>
+      </c>
+      <c r="C69" t="s">
+        <v>29</v>
+      </c>
+      <c r="D69" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69">
+        <v>-6200</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>45724</v>
+      </c>
+      <c r="C70" t="s">
+        <v>29</v>
+      </c>
+      <c r="D70" t="s">
+        <v>35</v>
+      </c>
+      <c r="E70">
+        <v>-3200</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>45723</v>
+      </c>
+      <c r="C71" t="s">
+        <v>29</v>
+      </c>
+      <c r="D71" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71">
+        <v>-8200</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>45724</v>
+      </c>
+      <c r="C72" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" t="s">
+        <v>37</v>
+      </c>
+      <c r="E72">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B73" s="2">
+        <v>45661</v>
+      </c>
+      <c r="C73" t="s">
+        <v>28</v>
+      </c>
+      <c r="D73" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73">
+        <v>-469</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B74" s="2">
+        <v>45662</v>
+      </c>
+      <c r="C74" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74">
+        <v>-244</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B75" s="2">
+        <v>45663</v>
+      </c>
+      <c r="C75" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75">
+        <v>-337</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B76" s="2">
+        <v>45664</v>
+      </c>
+      <c r="C76" t="s">
+        <v>28</v>
+      </c>
+      <c r="D76" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76">
+        <v>-310</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B77" s="2">
+        <v>45665</v>
+      </c>
+      <c r="C77" t="s">
+        <v>28</v>
+      </c>
+      <c r="D77" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77">
+        <v>-130</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B78" s="2">
+        <v>45666</v>
+      </c>
+      <c r="C78" t="s">
+        <v>28</v>
+      </c>
+      <c r="D78" t="s">
+        <v>3</v>
+      </c>
+      <c r="E78">
+        <v>-293</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B79" s="2">
+        <v>45667</v>
+      </c>
+      <c r="C79" t="s">
+        <v>28</v>
+      </c>
+      <c r="D79" t="s">
+        <v>3</v>
+      </c>
+      <c r="E79">
+        <v>-293</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B80" s="2">
+        <v>45668</v>
+      </c>
+      <c r="C80" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80">
+        <v>-293</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B81" s="2">
+        <v>45669</v>
+      </c>
+      <c r="C81" t="s">
+        <v>28</v>
+      </c>
+      <c r="D81" t="s">
         <v>5</v>
       </c>
-      <c r="D43" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43">
+      <c r="E81">
         <v>-195</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B82" s="2">
+        <v>45670</v>
+      </c>
+      <c r="C82" t="s">
+        <v>28</v>
+      </c>
+      <c r="D82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82">
+        <v>-325</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B83" s="2">
+        <v>45671</v>
+      </c>
+      <c r="C83" t="s">
+        <v>28</v>
+      </c>
+      <c r="D83" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83">
+        <v>-209</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B84" s="2">
+        <v>45672</v>
+      </c>
+      <c r="C84" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E84">
+        <v>-130</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B85" s="2">
+        <v>45673</v>
+      </c>
+      <c r="C85" t="s">
+        <v>28</v>
+      </c>
+      <c r="D85" t="s">
+        <v>5</v>
+      </c>
+      <c r="E85">
+        <v>-209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>